<commit_message>
Nom added to WiT
</commit_message>
<xml_diff>
--- a/Docs/Presentations/Slides/WiT.xlsx
+++ b/Docs/Presentations/Slides/WiT.xlsx
@@ -12,8 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11850" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Customer Reqs" sheetId="1" r:id="rId1"/>
+    <sheet name="Build Params" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>Design for existing liquid fuel engine</t>
   </si>
@@ -95,24 +95,166 @@
     <t>No. of Blades Z</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Impeller Discharge Angle </t>
-    </r>
-    <r>
-      <rPr>
+    <t>Performance parameters of EFS partial emission pump</t>
+  </si>
+  <si>
+    <t>Q (G.P.M)</t>
+  </si>
+  <si>
+    <t>H (ft)</t>
+  </si>
+  <si>
+    <t>P (KW)</t>
+  </si>
+  <si>
+    <t>≤ 3.5</t>
+  </si>
+  <si>
+    <t>Impeller Discharge Angle β(̊)</t>
+  </si>
+  <si>
+    <r>
+      <t>Impeller Outlet Diameter D</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Mathcad UniMath"/>
-        <family val="3"/>
-      </rPr>
-      <t>β(̊)</t>
-    </r>
-  </si>
-  <si>
-    <t>Base Diameter of Volute Caseing D3(in)</t>
-  </si>
-  <si>
-    <t>Length of Diffuser section LD(in)</t>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(in)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Impeller Blade width b</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(in)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Discharge Throat Diameter d</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(in)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Impeller eye Diameter D</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>e</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(in)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Base Diameter of Volute Caseing D</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(in)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Length of Diffuser section L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>D</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(in)</t>
+    </r>
   </si>
   <si>
     <r>
@@ -120,59 +262,53 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>α</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Mathcad UniMath"/>
-        <family val="3"/>
-      </rPr>
-      <t>α</t>
-    </r>
-    <r>
-      <rPr>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(̊)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>N</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>(</t>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>r</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Mathcad UniMath"/>
-        <family val="3"/>
-      </rPr>
-      <t>̊</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <t>Impeller eye Diameter De(in)</t>
-  </si>
-  <si>
-    <t>Discharge Throat Diameter d1(in)</t>
-  </si>
-  <si>
-    <t>Impeller Blade width b2(in)</t>
-  </si>
-  <si>
-    <t>Impeller Outlet Diameter D2(in)</t>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (r/min)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,14 +370,35 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Mathcad UniMath"/>
-      <family val="3"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -293,7 +450,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -334,6 +491,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
@@ -349,17 +508,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -653,17 +824,17 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:11" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="2:11" ht="5.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -679,20 +850,20 @@
       <c r="K4" s="6"/>
     </row>
     <row r="5" spans="2:11" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
       <c r="F5" s="11"/>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
     </row>
     <row r="6" spans="2:11" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="12"/>
@@ -707,20 +878,20 @@
       <c r="K6" s="14"/>
     </row>
     <row r="7" spans="2:11" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
       <c r="F7" s="11"/>
-      <c r="G7" s="18" t="s">
+      <c r="G7" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
     </row>
     <row r="8" spans="2:11" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="12"/>
@@ -735,20 +906,20 @@
       <c r="K8" s="14"/>
     </row>
     <row r="9" spans="2:11" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
       <c r="F9" s="11"/>
-      <c r="G9" s="18" t="s">
+      <c r="G9" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
     </row>
     <row r="10" spans="2:11" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="12"/>
@@ -763,20 +934,20 @@
       <c r="K10" s="14"/>
     </row>
     <row r="11" spans="2:11" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
       <c r="F11" s="11"/>
-      <c r="G11" s="18" t="s">
+      <c r="G11" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
     </row>
     <row r="12" spans="2:11" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="15"/>
@@ -791,20 +962,20 @@
       <c r="K12" s="14"/>
     </row>
     <row r="13" spans="2:11" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
       <c r="F13" s="11"/>
-      <c r="G13" s="18" t="s">
+      <c r="G13" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="8"/>
@@ -935,181 +1106,337 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:G19"/>
+  <dimension ref="B2:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:E13"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="7" width="15.85546875" customWidth="1"/>
+    <col min="3" max="5" width="14.5703125" customWidth="1"/>
+    <col min="6" max="7" width="7.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C3" s="21" t="s">
+    <row r="2" spans="2:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+    </row>
+    <row r="3" spans="2:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="16"/>
+      <c r="C3" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-    </row>
-    <row r="4" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="3:7" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="23" t="s">
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+    </row>
+    <row r="4" spans="2:9" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="16"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+    </row>
+    <row r="5" spans="2:9" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="16"/>
+      <c r="C5" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="24" t="s">
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="24"/>
-    </row>
-    <row r="6" spans="3:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-    </row>
-    <row r="7" spans="3:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="22" t="s">
+      <c r="G5" s="28"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+    </row>
+    <row r="6" spans="2:9" ht="4.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="16"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+    </row>
+    <row r="7" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="16"/>
+      <c r="C7" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="25">
+        <v>2.1</v>
+      </c>
+      <c r="G7" s="25"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+    </row>
+    <row r="8" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="16"/>
+      <c r="C8" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="21">
-        <v>2.1</v>
-      </c>
-      <c r="G7" s="21"/>
-    </row>
-    <row r="8" spans="3:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="21">
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="25">
         <v>0.2</v>
       </c>
-      <c r="G8" s="21"/>
-    </row>
-    <row r="9" spans="3:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="21" t="s">
+      <c r="G8" s="25"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+    </row>
+    <row r="9" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="16"/>
+      <c r="C9" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25">
+        <v>0.18</v>
+      </c>
+      <c r="G9" s="25"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+    </row>
+    <row r="10" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="16"/>
+      <c r="C10" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="25">
+        <v>0.43</v>
+      </c>
+      <c r="G10" s="25"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+    </row>
+    <row r="11" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="16"/>
+      <c r="C11" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="25">
+        <v>10</v>
+      </c>
+      <c r="G11" s="25"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+    </row>
+    <row r="12" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="16"/>
+      <c r="C12" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21">
-        <v>0.18</v>
-      </c>
-      <c r="G9" s="21"/>
-    </row>
-    <row r="10" spans="3:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="22" t="s">
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="25">
+        <v>36</v>
+      </c>
+      <c r="G12" s="25"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+    </row>
+    <row r="13" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="16"/>
+      <c r="C13" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="25">
+        <v>2.42</v>
+      </c>
+      <c r="G13" s="25"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+    </row>
+    <row r="14" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="16"/>
+      <c r="C14" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="25">
+        <v>1.2</v>
+      </c>
+      <c r="G14" s="25"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+    </row>
+    <row r="15" spans="2:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="16"/>
+      <c r="C15" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30">
+        <v>8</v>
+      </c>
+      <c r="G15" s="30"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+    </row>
+    <row r="16" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="16"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="16"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+    </row>
+    <row r="18" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="16"/>
+      <c r="C18" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+    </row>
+    <row r="19" spans="2:9" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+    </row>
+    <row r="20" spans="2:9" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="16"/>
+      <c r="C20" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="28"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+    </row>
+    <row r="21" spans="2:9" ht="4.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="16"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="16"/>
+      <c r="C22" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="25">
+        <v>12</v>
+      </c>
+      <c r="G22" s="25"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="16"/>
+      <c r="C23" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="25">
+        <v>754</v>
+      </c>
+      <c r="G23" s="25"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+    </row>
+    <row r="24" spans="2:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B24" s="16"/>
+      <c r="C24" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25">
+        <v>20500</v>
+      </c>
+      <c r="G24" s="25"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="16"/>
+      <c r="C25" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="21">
-        <v>0.43</v>
-      </c>
-      <c r="G10" s="21"/>
-    </row>
-    <row r="11" spans="3:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="21">
-        <v>10</v>
-      </c>
-      <c r="G11" s="21"/>
-    </row>
-    <row r="12" spans="3:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="21">
-        <v>36</v>
-      </c>
-      <c r="G12" s="21"/>
-    </row>
-    <row r="13" spans="3:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="21">
-        <v>2.42</v>
-      </c>
-      <c r="G13" s="21"/>
-    </row>
-    <row r="14" spans="3:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="21">
-        <v>1.2</v>
-      </c>
-      <c r="G14" s="21"/>
-    </row>
-    <row r="15" spans="3:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21">
-        <v>8</v>
-      </c>
-      <c r="G15" s="21"/>
-    </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-    </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-    </row>
+      <c r="G25" s="23"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+    </row>
+    <row r="26" spans="2:9" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="C9:E9"/>
+  <mergeCells count="36">
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="C15:E15"/>
     <mergeCell ref="C16:E16"/>
     <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C19:E19"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="F9:G9"/>
@@ -1120,11 +1447,27 @@
     <mergeCell ref="C10:E10"/>
     <mergeCell ref="C13:E13"/>
     <mergeCell ref="C14:E14"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="C9:E9"/>
     <mergeCell ref="C5:E5"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="C3:G3"/>
     <mergeCell ref="C6:E6"/>
     <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="F24:G24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added more photos to pub
</commit_message>
<xml_diff>
--- a/Docs/Presentations/Slides/WiT.xlsx
+++ b/Docs/Presentations/Slides/WiT.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11850" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11850" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Customer Reqs" sheetId="1" r:id="rId1"/>
     <sheet name="Build Params" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
   <si>
     <t>Design for existing liquid fuel engine</t>
   </si>
@@ -303,12 +304,72 @@
       <t xml:space="preserve"> (r/min)</t>
     </r>
   </si>
+  <si>
+    <t>Summary of monitored variables</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Monitoring device</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>Coupled to motor shaft</t>
+  </si>
+  <si>
+    <t>Required electric power</t>
+  </si>
+  <si>
+    <t>Sensing simultaneously motor current and voltage</t>
+  </si>
+  <si>
+    <t>Pressure Transducer</t>
+  </si>
+  <si>
+    <t>Pump Inlet Temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pump Inlet/Outlet Pressure </t>
+  </si>
+  <si>
+    <t>K-Type Thermocouple</t>
+  </si>
+  <si>
+    <t>Pump Rotational Speed</t>
+  </si>
+  <si>
+    <t>Homebrew Optical Sensor</t>
+  </si>
+  <si>
+    <t>Pump Torque</t>
+  </si>
+  <si>
+    <t>Load Cell</t>
+  </si>
+  <si>
+    <t>Coupled to free-floating torque arm</t>
+  </si>
+  <si>
+    <t>Liquid Turbine Flow Meter</t>
+  </si>
+  <si>
+    <t>Indicates possible cavitation</t>
+  </si>
+  <si>
+    <t>Pump Flow Rate</t>
+  </si>
+  <si>
+    <t>Indirect Measure</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -400,6 +461,39 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Garamond"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Garamond"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Garamond"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Garamond"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -409,7 +503,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -446,11 +540,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -508,33 +625,64 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1108,7 +1256,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
@@ -1130,13 +1278,13 @@
     </row>
     <row r="3" spans="2:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="16"/>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
       <c r="H3" s="16"/>
       <c r="I3" s="16"/>
     </row>
@@ -1166,9 +1314,9 @@
     </row>
     <row r="6" spans="2:9" ht="4.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B6" s="16"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
       <c r="H6" s="16"/>
@@ -1176,135 +1324,135 @@
     </row>
     <row r="7" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="16"/>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="25">
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="24">
         <v>2.1</v>
       </c>
-      <c r="G7" s="25"/>
+      <c r="G7" s="24"/>
       <c r="H7" s="16"/>
       <c r="I7" s="16"/>
     </row>
     <row r="8" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="16"/>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="25">
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="24">
         <v>0.2</v>
       </c>
-      <c r="G8" s="25"/>
+      <c r="G8" s="24"/>
       <c r="H8" s="16"/>
       <c r="I8" s="16"/>
     </row>
     <row r="9" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="16"/>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25">
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24">
         <v>0.18</v>
       </c>
-      <c r="G9" s="25"/>
+      <c r="G9" s="24"/>
       <c r="H9" s="16"/>
       <c r="I9" s="16"/>
     </row>
     <row r="10" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="16"/>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="25">
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="24">
         <v>0.43</v>
       </c>
-      <c r="G10" s="25"/>
+      <c r="G10" s="24"/>
       <c r="H10" s="16"/>
       <c r="I10" s="16"/>
     </row>
     <row r="11" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="16"/>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="25">
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="24">
         <v>10</v>
       </c>
-      <c r="G11" s="25"/>
+      <c r="G11" s="24"/>
       <c r="H11" s="16"/>
       <c r="I11" s="16"/>
     </row>
     <row r="12" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="16"/>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="25">
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="24">
         <v>36</v>
       </c>
-      <c r="G12" s="25"/>
+      <c r="G12" s="24"/>
       <c r="H12" s="16"/>
       <c r="I12" s="16"/>
     </row>
     <row r="13" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="16"/>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="25">
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="24">
         <v>2.42</v>
       </c>
-      <c r="G13" s="25"/>
+      <c r="G13" s="24"/>
       <c r="H13" s="16"/>
       <c r="I13" s="16"/>
     </row>
     <row r="14" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="16"/>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="25">
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="24">
         <v>1.2</v>
       </c>
-      <c r="G14" s="25"/>
+      <c r="G14" s="24"/>
       <c r="H14" s="16"/>
       <c r="I14" s="16"/>
     </row>
     <row r="15" spans="2:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="16"/>
-      <c r="C15" s="30" t="s">
+      <c r="C15" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30">
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25">
         <v>8</v>
       </c>
-      <c r="G15" s="30"/>
+      <c r="G15" s="25"/>
       <c r="H15" s="16"/>
       <c r="I15" s="16"/>
     </row>
     <row r="16" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B16" s="16"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
       <c r="F16" s="16"/>
       <c r="G16" s="16"/>
       <c r="H16" s="16"/>
@@ -1312,9 +1460,9 @@
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="16"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
       <c r="F17" s="16"/>
       <c r="G17" s="16"/>
       <c r="H17" s="16"/>
@@ -1322,13 +1470,13 @@
     </row>
     <row r="18" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="16"/>
-      <c r="C18" s="26" t="s">
+      <c r="C18" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
       <c r="H18" s="16"/>
       <c r="I18" s="16"/>
     </row>
@@ -1358,9 +1506,9 @@
     </row>
     <row r="21" spans="2:9" ht="4.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B21" s="16"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="29"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
       <c r="F21" s="16"/>
       <c r="G21" s="16"/>
       <c r="H21" s="16"/>
@@ -1368,57 +1516,57 @@
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="16"/>
-      <c r="C22" s="24" t="s">
+      <c r="C22" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="25">
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="24">
         <v>12</v>
       </c>
-      <c r="G22" s="25"/>
+      <c r="G22" s="24"/>
       <c r="H22" s="16"/>
       <c r="I22" s="16"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="16"/>
-      <c r="C23" s="24" t="s">
+      <c r="C23" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="25">
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="24">
         <v>754</v>
       </c>
-      <c r="G23" s="25"/>
+      <c r="G23" s="24"/>
       <c r="H23" s="16"/>
       <c r="I23" s="16"/>
     </row>
     <row r="24" spans="2:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B24" s="16"/>
-      <c r="C24" s="25" t="s">
+      <c r="C24" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25">
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24">
         <v>20500</v>
       </c>
-      <c r="G24" s="25"/>
+      <c r="G24" s="24"/>
       <c r="H24" s="16"/>
       <c r="I24" s="16"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="16"/>
-      <c r="C25" s="23" t="s">
+      <c r="C25" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23" t="s">
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="G25" s="23"/>
+      <c r="G25" s="26"/>
       <c r="H25" s="16"/>
       <c r="I25" s="16"/>
     </row>
@@ -1432,42 +1580,190 @@
     <row r="27" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="F24:G24"/>
     <mergeCell ref="C18:G18"/>
     <mergeCell ref="C20:E20"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="C21:E21"/>
     <mergeCell ref="C22:E22"/>
     <mergeCell ref="F22:G22"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:H13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="5" width="29.28515625" customWidth="1"/>
+    <col min="6" max="6" width="36" customWidth="1"/>
+    <col min="7" max="7" width="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+    </row>
+    <row r="3" spans="3:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C3" s="32"/>
+      <c r="D3" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="32"/>
+    </row>
+    <row r="4" spans="3:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="32"/>
+      <c r="G4" s="33"/>
+    </row>
+    <row r="5" spans="3:8" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="32"/>
+      <c r="D5" s="41" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="34"/>
+      <c r="H5" s="31"/>
+    </row>
+    <row r="6" spans="3:8" ht="48.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="42"/>
+      <c r="D6" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="37"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="31"/>
+    </row>
+    <row r="7" spans="3:8" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="42"/>
+      <c r="D7" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="39"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="31"/>
+    </row>
+    <row r="8" spans="3:8" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="32"/>
+      <c r="D8" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="34"/>
+      <c r="H8" s="31"/>
+    </row>
+    <row r="9" spans="3:8" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="32"/>
+      <c r="D9" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="34"/>
+      <c r="H9" s="31"/>
+    </row>
+    <row r="10" spans="3:8" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="32"/>
+      <c r="D10" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" s="34"/>
+      <c r="H10" s="31"/>
+    </row>
+    <row r="11" spans="3:8" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="32"/>
+      <c r="D11" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" s="32"/>
+    </row>
+    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+    </row>
+    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C13" s="32"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D3:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>